<commit_message>
First commit - add index.html và data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LearningSpace\dannyGreen_livestreamdeal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B201A0C-0257-4CFD-953D-75B8E70F891E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92572939-4CE0-4638-A557-8AA688F7BAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD7A8270-FB9B-4B81-9199-B40BD875551E}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11160" xr2:uid="{AD7A8270-FB9B-4B81-9199-B40BD875551E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -139,9 +139,6 @@
     <t>212.000</t>
   </si>
   <si>
-    <t>20%</t>
-  </si>
-  <si>
     <t>329.000</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>235.000</t>
   </si>
   <si>
-    <t>10%</t>
-  </si>
-  <si>
     <t>294.000</t>
   </si>
   <si>
@@ -326,6 +320,12 @@
   </si>
   <si>
     <t>https://down-vn.img.susercontent.com/file/vn-11134207-820l4-mdvkvokxfr460b.webp</t>
+  </si>
+  <si>
+    <t>-20%</t>
+  </si>
+  <si>
+    <t>-10%</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -403,6 +403,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -718,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0496FC-16B7-4A21-8716-53BF8FEFD78D}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,7 +778,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -795,138 +796,138 @@
         <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>34</v>
+        <v>95</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>18</v>
@@ -935,33 +936,33 @@
         <v>12</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>18</v>
@@ -970,33 +971,33 @@
         <v>12</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>21</v>
@@ -1005,33 +1006,33 @@
         <v>12</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>21</v>
@@ -1040,33 +1041,33 @@
         <v>12</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>24</v>
@@ -1075,30 +1076,30 @@
         <v>14</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>24</v>
@@ -1107,30 +1108,30 @@
         <v>14</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>24</v>
@@ -1139,30 +1140,30 @@
         <v>14</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>24</v>
@@ -1171,30 +1172,30 @@
         <v>14</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>24</v>
@@ -1203,30 +1204,30 @@
         <v>14</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>38</v>
+        <v>96</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>24</v>
@@ -1235,8 +1236,260 @@
         <v>14</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H59" s="5"/>
+    </row>
+    <row r="60" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H67" s="5"/>
+    </row>
+    <row r="68" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H68" s="5"/>
+    </row>
+    <row r="69" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H70" s="5"/>
+    </row>
+    <row r="71" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H71" s="5"/>
+    </row>
+    <row r="72" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H73" s="5"/>
+    </row>
+    <row r="74" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H74" s="5"/>
+    </row>
+    <row r="75" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H75" s="5"/>
+    </row>
+    <row r="76" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H76" s="5"/>
+    </row>
+    <row r="77" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H77" s="5"/>
+    </row>
+    <row r="78" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H78" s="5"/>
+    </row>
+    <row r="79" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H79" s="5"/>
+    </row>
+    <row r="80" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H84" s="5"/>
+    </row>
+    <row r="85" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H87" s="5"/>
+    </row>
+    <row r="88" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H89" s="5"/>
+    </row>
+    <row r="90" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H90" s="5"/>
+    </row>
+    <row r="91" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H91" s="5"/>
+    </row>
+    <row r="92" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H92" s="5"/>
+    </row>
+    <row r="93" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H93" s="5"/>
+    </row>
+    <row r="94" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H94" s="5"/>
+    </row>
+    <row r="95" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H95" s="5"/>
+    </row>
+    <row r="96" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H96" s="5"/>
+    </row>
+    <row r="97" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H97" s="5"/>
+    </row>
+    <row r="98" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H98" s="5"/>
+    </row>
+    <row r="99" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H99" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>